<commit_message>
update v3 swap method SA
</commit_message>
<xml_diff>
--- a/src/data_uisi.xlsx
+++ b/src/data_uisi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acern\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E8D1A3-6025-4180-808E-842976C7C9B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19E07CC-D650-40A0-B6D5-46F619857CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{35A121DA-9B65-45CA-BEBF-895C36E667B5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{35A121DA-9B65-45CA-BEBF-895C36E667B5}"/>
   </bookViews>
   <sheets>
     <sheet name="ruangan" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3972" uniqueCount="921">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3972" uniqueCount="920">
   <si>
     <t>B2-R1</t>
   </si>
@@ -2798,16 +2798,13 @@
     <t>yes</t>
   </si>
   <si>
-    <t>B2-R1, B3-R1, B3-R2, B3R3, CM-101, CM-102, CM-103, CM-201, CM-202, CM-203, CM-204, CM-205, CM-208, G2-R2, G2-R3, G2-R4, G2-R5, G2-R6, G2-R7, G3-R1, G3-R2, G3-R3, G3-R4, G4-R1, G4-R2, G4-R3, G4-R4</t>
-  </si>
-  <si>
     <t>Peserta</t>
   </si>
   <si>
-    <t>CM-206, CM-207, CM-LabVirtual, CM-Lab3, G5-Lab1, G5-Lab2</t>
-  </si>
-  <si>
     <t>monday</t>
+  </si>
+  <si>
+    <t>B2-R1, B3-R1, B3-R2, B3R3, CM-101, CM-102, CM-103, CM-201, CM-202, CM-203, CM-204, CM-205, CM-208, G2-R2, G2-R3, G2-R4, G2-R5, G2-R6, G2-R7, G3-R1, G3-R2, G3-R3, G3-R4, G4-R1, G4-R2, G4-R3, G4-R4, CM-206, CM-207, CM-LabVirtual, CM-Lab3, G5-Lab1, G5-Lab2</t>
   </si>
 </sst>
 </file>
@@ -3174,7 +3171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="226">
+  <cellXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3756,9 +3753,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5158,7 +5152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84397B3-03F7-4516-8818-17F518B1BA4E}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B50" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
@@ -6167,7 +6161,7 @@
         <v>290</v>
       </c>
       <c r="E44" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -6213,7 +6207,7 @@
         <v>288</v>
       </c>
       <c r="E46" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -6282,7 +6276,7 @@
         <v>291</v>
       </c>
       <c r="E49" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -6558,7 +6552,7 @@
         <v>291</v>
       </c>
       <c r="E61" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="F61">
         <v>0</v>
@@ -6604,7 +6598,7 @@
         <v>289</v>
       </c>
       <c r="E63" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="F63">
         <v>0</v>
@@ -7067,7 +7061,7 @@
         <v>289</v>
       </c>
       <c r="E83" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="F83">
         <v>0</v>
@@ -7435,8 +7429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D683433F-DAFA-4342-BB02-72627F55AF9D}">
   <dimension ref="A1:N374"/>
   <sheetViews>
-    <sheetView topLeftCell="D308" workbookViewId="0">
-      <selection activeCell="N358" sqref="N358"/>
+    <sheetView tabSelected="1" topLeftCell="E355" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N374"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7473,7 +7467,7 @@
         <v>900</v>
       </c>
       <c r="G1" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="H1" t="s">
         <v>898</v>
@@ -7534,7 +7528,7 @@
         <v>915</v>
       </c>
       <c r="N2" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -7574,7 +7568,7 @@
         <v>915</v>
       </c>
       <c r="N3" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -7612,7 +7606,7 @@
         <v>915</v>
       </c>
       <c r="N4" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -7650,7 +7644,7 @@
         <v>915</v>
       </c>
       <c r="N5" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -7690,7 +7684,7 @@
         <v>915</v>
       </c>
       <c r="N6" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -7730,7 +7724,7 @@
         <v>915</v>
       </c>
       <c r="N7" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -7768,7 +7762,7 @@
         <v>915</v>
       </c>
       <c r="N8" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -7808,7 +7802,7 @@
         <v>915</v>
       </c>
       <c r="N9" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -7846,7 +7840,7 @@
         <v>915</v>
       </c>
       <c r="N10" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -7886,7 +7880,7 @@
         <v>915</v>
       </c>
       <c r="N11" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -7924,7 +7918,7 @@
         <v>915</v>
       </c>
       <c r="N12" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -7962,7 +7956,7 @@
         <v>915</v>
       </c>
       <c r="N13" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -7998,7 +7992,7 @@
         <v>915</v>
       </c>
       <c r="N14" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -8038,7 +8032,7 @@
         <v>915</v>
       </c>
       <c r="N15" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -8078,7 +8072,7 @@
         <v>915</v>
       </c>
       <c r="N16" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -8116,7 +8110,7 @@
         <v>915</v>
       </c>
       <c r="N17" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -8154,7 +8148,7 @@
         <v>915</v>
       </c>
       <c r="N18" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -8192,7 +8186,7 @@
         <v>915</v>
       </c>
       <c r="N19" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -8230,7 +8224,7 @@
         <v>915</v>
       </c>
       <c r="N20" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -8268,7 +8262,7 @@
         <v>915</v>
       </c>
       <c r="N21" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -8306,7 +8300,7 @@
         <v>915</v>
       </c>
       <c r="N22" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -8344,7 +8338,7 @@
         <v>915</v>
       </c>
       <c r="N23" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -8382,7 +8376,7 @@
         <v>915</v>
       </c>
       <c r="N24" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -8420,7 +8414,7 @@
         <v>915</v>
       </c>
       <c r="N25" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -8458,7 +8452,7 @@
         <v>915</v>
       </c>
       <c r="N26" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -8496,7 +8490,7 @@
         <v>915</v>
       </c>
       <c r="N27" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -8534,7 +8528,7 @@
         <v>915</v>
       </c>
       <c r="N28" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -8572,7 +8566,7 @@
         <v>915</v>
       </c>
       <c r="N29" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -8610,7 +8604,7 @@
         <v>915</v>
       </c>
       <c r="N30" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -8648,7 +8642,7 @@
         <v>915</v>
       </c>
       <c r="N31" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -8686,7 +8680,7 @@
         <v>915</v>
       </c>
       <c r="N32" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -8724,7 +8718,7 @@
         <v>915</v>
       </c>
       <c r="N33" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -8762,7 +8756,7 @@
         <v>915</v>
       </c>
       <c r="N34" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -8798,7 +8792,7 @@
         <v>915</v>
       </c>
       <c r="N35" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -8834,7 +8828,7 @@
         <v>915</v>
       </c>
       <c r="N36" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -8872,7 +8866,7 @@
         <v>915</v>
       </c>
       <c r="N37" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="38" spans="1:14">
@@ -8910,7 +8904,7 @@
         <v>915</v>
       </c>
       <c r="N38" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="39" spans="1:14">
@@ -8948,7 +8942,7 @@
         <v>915</v>
       </c>
       <c r="N39" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="40" spans="1:14">
@@ -8986,7 +8980,7 @@
         <v>915</v>
       </c>
       <c r="N40" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="41" spans="1:14">
@@ -9024,7 +9018,7 @@
         <v>915</v>
       </c>
       <c r="N41" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="42" spans="1:14">
@@ -9062,7 +9056,7 @@
         <v>915</v>
       </c>
       <c r="N42" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="43" spans="1:14">
@@ -9100,7 +9094,7 @@
         <v>915</v>
       </c>
       <c r="N43" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -9138,7 +9132,7 @@
         <v>915</v>
       </c>
       <c r="N44" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="45" spans="1:14">
@@ -9176,7 +9170,7 @@
         <v>915</v>
       </c>
       <c r="N45" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="46" spans="1:14">
@@ -9214,7 +9208,7 @@
         <v>915</v>
       </c>
       <c r="N46" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="47" spans="1:14">
@@ -9252,7 +9246,7 @@
         <v>915</v>
       </c>
       <c r="N47" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="48" spans="1:14">
@@ -9292,7 +9286,7 @@
         <v>915</v>
       </c>
       <c r="N48" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="49" spans="1:14">
@@ -9330,7 +9324,7 @@
         <v>915</v>
       </c>
       <c r="N49" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="50" spans="1:14">
@@ -9368,7 +9362,7 @@
         <v>915</v>
       </c>
       <c r="N50" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="51" spans="1:14">
@@ -9406,7 +9400,7 @@
         <v>915</v>
       </c>
       <c r="N51" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="52" spans="1:14">
@@ -9444,7 +9438,7 @@
         <v>915</v>
       </c>
       <c r="N52" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="53" spans="1:14">
@@ -9482,7 +9476,7 @@
         <v>915</v>
       </c>
       <c r="N53" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="54" spans="1:14">
@@ -9520,7 +9514,7 @@
         <v>915</v>
       </c>
       <c r="N54" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="55" spans="1:14">
@@ -9558,7 +9552,7 @@
         <v>915</v>
       </c>
       <c r="N55" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="56" spans="1:14">
@@ -9596,7 +9590,7 @@
         <v>915</v>
       </c>
       <c r="N56" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="57" spans="1:14">
@@ -9634,7 +9628,7 @@
         <v>915</v>
       </c>
       <c r="N57" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="58" spans="1:14">
@@ -9672,7 +9666,7 @@
         <v>915</v>
       </c>
       <c r="N58" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="59" spans="1:14">
@@ -9710,7 +9704,7 @@
         <v>915</v>
       </c>
       <c r="N59" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="60" spans="1:14">
@@ -9748,7 +9742,7 @@
         <v>915</v>
       </c>
       <c r="N60" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="61" spans="1:14">
@@ -9786,7 +9780,7 @@
         <v>915</v>
       </c>
       <c r="N61" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="62" spans="1:14">
@@ -9824,7 +9818,7 @@
         <v>915</v>
       </c>
       <c r="N62" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="63" spans="1:14">
@@ -9862,7 +9856,7 @@
         <v>915</v>
       </c>
       <c r="N63" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="64" spans="1:14">
@@ -9900,7 +9894,7 @@
         <v>915</v>
       </c>
       <c r="N64" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="65" spans="1:14">
@@ -9938,7 +9932,7 @@
         <v>915</v>
       </c>
       <c r="N65" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="66" spans="1:14">
@@ -9976,7 +9970,7 @@
         <v>915</v>
       </c>
       <c r="N66" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="67" spans="1:14">
@@ -10014,7 +10008,7 @@
         <v>915</v>
       </c>
       <c r="N67" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="68" spans="1:14">
@@ -10052,7 +10046,7 @@
         <v>915</v>
       </c>
       <c r="N68" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="69" spans="1:14">
@@ -10090,7 +10084,7 @@
         <v>915</v>
       </c>
       <c r="N69" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="70" spans="1:14">
@@ -10128,7 +10122,7 @@
         <v>915</v>
       </c>
       <c r="N70" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="71" spans="1:14">
@@ -10166,7 +10160,7 @@
         <v>915</v>
       </c>
       <c r="N71" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="72" spans="1:14">
@@ -10204,7 +10198,7 @@
         <v>915</v>
       </c>
       <c r="N72" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="73" spans="1:14">
@@ -10242,7 +10236,7 @@
         <v>915</v>
       </c>
       <c r="N73" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="74" spans="1:14">
@@ -10280,7 +10274,7 @@
         <v>915</v>
       </c>
       <c r="N74" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="75" spans="1:14">
@@ -10316,7 +10310,7 @@
         <v>915</v>
       </c>
       <c r="N75" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="76" spans="1:14">
@@ -10354,7 +10348,7 @@
         <v>915</v>
       </c>
       <c r="N76" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="77" spans="1:14">
@@ -10390,7 +10384,7 @@
         <v>915</v>
       </c>
       <c r="N77" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="78" spans="1:14">
@@ -10428,7 +10422,7 @@
         <v>915</v>
       </c>
       <c r="N78" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="79" spans="1:14">
@@ -10466,7 +10460,7 @@
         <v>915</v>
       </c>
       <c r="N79" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="80" spans="1:14">
@@ -10504,7 +10498,7 @@
         <v>915</v>
       </c>
       <c r="N80" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="81" spans="1:14">
@@ -10542,7 +10536,7 @@
         <v>915</v>
       </c>
       <c r="N81" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="82" spans="1:14">
@@ -10580,7 +10574,7 @@
         <v>915</v>
       </c>
       <c r="N82" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="83" spans="1:14">
@@ -10618,7 +10612,7 @@
         <v>915</v>
       </c>
       <c r="N83" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="84" spans="1:14">
@@ -10656,7 +10650,7 @@
         <v>915</v>
       </c>
       <c r="N84" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="85" spans="1:14">
@@ -10694,7 +10688,7 @@
         <v>915</v>
       </c>
       <c r="N85" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="86" spans="1:14">
@@ -10732,7 +10726,7 @@
         <v>915</v>
       </c>
       <c r="N86" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="87" spans="1:14">
@@ -10770,7 +10764,7 @@
         <v>915</v>
       </c>
       <c r="N87" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="88" spans="1:14">
@@ -10808,7 +10802,7 @@
         <v>915</v>
       </c>
       <c r="N88" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="89" spans="1:14">
@@ -10846,7 +10840,7 @@
         <v>915</v>
       </c>
       <c r="N89" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="90" spans="1:14">
@@ -10884,7 +10878,7 @@
         <v>915</v>
       </c>
       <c r="N90" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="91" spans="1:14">
@@ -10922,7 +10916,7 @@
         <v>915</v>
       </c>
       <c r="N91" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="92" spans="1:14">
@@ -10960,7 +10954,7 @@
         <v>915</v>
       </c>
       <c r="N92" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="93" spans="1:14">
@@ -10998,7 +10992,7 @@
         <v>915</v>
       </c>
       <c r="N93" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="94" spans="1:14">
@@ -11036,7 +11030,7 @@
         <v>915</v>
       </c>
       <c r="N94" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="95" spans="1:14">
@@ -11074,7 +11068,7 @@
         <v>915</v>
       </c>
       <c r="N95" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="96" spans="1:14">
@@ -11150,7 +11144,7 @@
         <v>915</v>
       </c>
       <c r="N97" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="98" spans="1:14">
@@ -11188,7 +11182,7 @@
         <v>915</v>
       </c>
       <c r="N98" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="99" spans="1:14">
@@ -11226,7 +11220,7 @@
         <v>915</v>
       </c>
       <c r="N99" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="100" spans="1:14">
@@ -11264,7 +11258,7 @@
         <v>915</v>
       </c>
       <c r="N100" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="101" spans="1:14">
@@ -11302,7 +11296,7 @@
         <v>915</v>
       </c>
       <c r="N101" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="102" spans="1:14">
@@ -11340,7 +11334,7 @@
         <v>915</v>
       </c>
       <c r="N102" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="103" spans="1:14">
@@ -11416,7 +11410,7 @@
         <v>915</v>
       </c>
       <c r="N104" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="105" spans="1:14">
@@ -11452,7 +11446,7 @@
         <v>915</v>
       </c>
       <c r="N105" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="106" spans="1:14">
@@ -11488,7 +11482,7 @@
         <v>915</v>
       </c>
       <c r="N106" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="107" spans="1:14">
@@ -11526,7 +11520,7 @@
         <v>915</v>
       </c>
       <c r="N107" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="108" spans="1:14">
@@ -11564,7 +11558,7 @@
         <v>915</v>
       </c>
       <c r="N108" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="109" spans="1:14">
@@ -11602,7 +11596,7 @@
         <v>915</v>
       </c>
       <c r="N109" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="110" spans="1:14">
@@ -11640,7 +11634,7 @@
         <v>915</v>
       </c>
       <c r="N110" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="111" spans="1:14">
@@ -11678,7 +11672,7 @@
         <v>915</v>
       </c>
       <c r="N111" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="112" spans="1:14">
@@ -11716,7 +11710,7 @@
         <v>915</v>
       </c>
       <c r="N112" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="113" spans="1:14">
@@ -11754,7 +11748,7 @@
         <v>915</v>
       </c>
       <c r="N113" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="114" spans="1:14">
@@ -11792,7 +11786,7 @@
         <v>915</v>
       </c>
       <c r="N114" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="115" spans="1:14">
@@ -11830,7 +11824,7 @@
         <v>915</v>
       </c>
       <c r="N115" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="116" spans="1:14">
@@ -11868,7 +11862,7 @@
         <v>915</v>
       </c>
       <c r="N116" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="117" spans="1:14">
@@ -11906,7 +11900,7 @@
         <v>915</v>
       </c>
       <c r="N117" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="118" spans="1:14">
@@ -11944,7 +11938,7 @@
         <v>915</v>
       </c>
       <c r="N118" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="119" spans="1:14">
@@ -11982,7 +11976,7 @@
         <v>915</v>
       </c>
       <c r="N119" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="120" spans="1:14">
@@ -12020,7 +12014,7 @@
         <v>915</v>
       </c>
       <c r="N120" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="121" spans="1:14">
@@ -12058,7 +12052,7 @@
         <v>915</v>
       </c>
       <c r="N121" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="122" spans="1:14">
@@ -12096,7 +12090,7 @@
         <v>915</v>
       </c>
       <c r="N122" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="123" spans="1:14">
@@ -12134,7 +12128,7 @@
         <v>915</v>
       </c>
       <c r="N123" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="124" spans="1:14">
@@ -12172,7 +12166,7 @@
         <v>915</v>
       </c>
       <c r="N124" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="125" spans="1:14">
@@ -12210,7 +12204,7 @@
         <v>915</v>
       </c>
       <c r="N125" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="126" spans="1:14">
@@ -12248,7 +12242,7 @@
         <v>915</v>
       </c>
       <c r="N126" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="127" spans="1:14">
@@ -12284,7 +12278,7 @@
         <v>915</v>
       </c>
       <c r="N127" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="128" spans="1:14">
@@ -12322,7 +12316,7 @@
         <v>915</v>
       </c>
       <c r="N128" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="129" spans="1:14">
@@ -12360,7 +12354,7 @@
         <v>915</v>
       </c>
       <c r="N129" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="130" spans="1:14">
@@ -12398,7 +12392,7 @@
         <v>915</v>
       </c>
       <c r="N130" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="131" spans="1:14">
@@ -12436,7 +12430,7 @@
         <v>915</v>
       </c>
       <c r="N131" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="132" spans="1:14">
@@ -12472,7 +12466,7 @@
         <v>915</v>
       </c>
       <c r="N132" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="133" spans="1:14">
@@ -12510,7 +12504,7 @@
         <v>915</v>
       </c>
       <c r="N133" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="134" spans="1:14">
@@ -12548,7 +12542,7 @@
         <v>915</v>
       </c>
       <c r="N134" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="135" spans="1:14">
@@ -12586,7 +12580,7 @@
         <v>915</v>
       </c>
       <c r="N135" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="136" spans="1:14">
@@ -12662,7 +12656,7 @@
         <v>915</v>
       </c>
       <c r="N137" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="138" spans="1:14">
@@ -12700,7 +12694,7 @@
         <v>915</v>
       </c>
       <c r="N138" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="139" spans="1:14">
@@ -12738,7 +12732,7 @@
         <v>915</v>
       </c>
       <c r="N139" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="140" spans="1:14">
@@ -12776,7 +12770,7 @@
         <v>915</v>
       </c>
       <c r="N140" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="141" spans="1:14">
@@ -12814,7 +12808,7 @@
         <v>915</v>
       </c>
       <c r="N141" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="142" spans="1:14">
@@ -12852,7 +12846,7 @@
         <v>915</v>
       </c>
       <c r="N142" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="143" spans="1:14">
@@ -12890,7 +12884,7 @@
         <v>915</v>
       </c>
       <c r="N143" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="144" spans="1:14">
@@ -12928,7 +12922,7 @@
         <v>915</v>
       </c>
       <c r="N144" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="145" spans="1:14">
@@ -12966,7 +12960,7 @@
         <v>915</v>
       </c>
       <c r="N145" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="146" spans="1:14">
@@ -13004,7 +12998,7 @@
         <v>915</v>
       </c>
       <c r="N146" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="147" spans="1:14">
@@ -13042,7 +13036,7 @@
         <v>915</v>
       </c>
       <c r="N147" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="148" spans="1:14">
@@ -13080,7 +13074,7 @@
         <v>915</v>
       </c>
       <c r="N148" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="149" spans="1:14">
@@ -13115,7 +13109,7 @@
         <v>915</v>
       </c>
       <c r="N149" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="150" spans="1:14">
@@ -13153,7 +13147,7 @@
         <v>915</v>
       </c>
       <c r="N150" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="151" spans="1:14">
@@ -13188,7 +13182,7 @@
         <v>915</v>
       </c>
       <c r="N151" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="152" spans="1:14">
@@ -13224,7 +13218,7 @@
         <v>915</v>
       </c>
       <c r="N152" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="153" spans="1:14">
@@ -13262,7 +13256,7 @@
         <v>915</v>
       </c>
       <c r="N153" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="154" spans="1:14">
@@ -13300,7 +13294,7 @@
         <v>915</v>
       </c>
       <c r="N154" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="155" spans="1:14">
@@ -13338,7 +13332,7 @@
         <v>915</v>
       </c>
       <c r="N155" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="156" spans="1:14">
@@ -13414,7 +13408,7 @@
         <v>915</v>
       </c>
       <c r="N157" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="158" spans="1:14">
@@ -13452,7 +13446,7 @@
         <v>915</v>
       </c>
       <c r="N158" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="159" spans="1:14">
@@ -13490,7 +13484,7 @@
         <v>915</v>
       </c>
       <c r="N159" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="160" spans="1:14">
@@ -13528,7 +13522,7 @@
         <v>915</v>
       </c>
       <c r="N160" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="161" spans="1:14">
@@ -13564,7 +13558,7 @@
         <v>915</v>
       </c>
       <c r="N161" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="162" spans="1:14">
@@ -13602,7 +13596,7 @@
         <v>915</v>
       </c>
       <c r="N162" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="163" spans="1:14">
@@ -13640,7 +13634,7 @@
         <v>915</v>
       </c>
       <c r="N163" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="164" spans="1:14">
@@ -13678,7 +13672,7 @@
         <v>915</v>
       </c>
       <c r="N164" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="165" spans="1:14">
@@ -13714,7 +13708,7 @@
         <v>915</v>
       </c>
       <c r="N165" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="166" spans="1:14">
@@ -13750,7 +13744,7 @@
         <v>915</v>
       </c>
       <c r="N166" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="167" spans="1:14">
@@ -13784,7 +13778,7 @@
         <v>915</v>
       </c>
       <c r="N167" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="168" spans="1:14">
@@ -13822,7 +13816,7 @@
         <v>915</v>
       </c>
       <c r="N168" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="169" spans="1:14">
@@ -13860,7 +13854,7 @@
         <v>915</v>
       </c>
       <c r="N169" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="170" spans="1:14">
@@ -13898,7 +13892,7 @@
         <v>915</v>
       </c>
       <c r="N170" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="171" spans="1:14">
@@ -13936,7 +13930,7 @@
         <v>915</v>
       </c>
       <c r="N171" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="172" spans="1:14">
@@ -13974,7 +13968,7 @@
         <v>915</v>
       </c>
       <c r="N172" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="173" spans="1:14">
@@ -14012,7 +14006,7 @@
         <v>915</v>
       </c>
       <c r="N173" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="174" spans="1:14">
@@ -14050,7 +14044,7 @@
         <v>915</v>
       </c>
       <c r="N174" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="175" spans="1:14">
@@ -14088,7 +14082,7 @@
         <v>915</v>
       </c>
       <c r="N175" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="176" spans="1:14">
@@ -14126,7 +14120,7 @@
         <v>915</v>
       </c>
       <c r="N176" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="177" spans="1:14">
@@ -14164,7 +14158,7 @@
         <v>915</v>
       </c>
       <c r="N177" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="178" spans="1:14">
@@ -14202,7 +14196,7 @@
         <v>915</v>
       </c>
       <c r="N178" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="179" spans="1:14">
@@ -14240,7 +14234,7 @@
         <v>915</v>
       </c>
       <c r="N179" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="180" spans="1:14">
@@ -14278,7 +14272,7 @@
         <v>915</v>
       </c>
       <c r="N180" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="181" spans="1:14">
@@ -14392,7 +14386,7 @@
         <v>915</v>
       </c>
       <c r="N183" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="184" spans="1:14">
@@ -14430,7 +14424,7 @@
         <v>915</v>
       </c>
       <c r="N184" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="185" spans="1:14">
@@ -14468,7 +14462,7 @@
         <v>915</v>
       </c>
       <c r="N185" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="186" spans="1:14">
@@ -14506,7 +14500,7 @@
         <v>915</v>
       </c>
       <c r="N186" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="187" spans="1:14">
@@ -14544,7 +14538,7 @@
         <v>915</v>
       </c>
       <c r="N187" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="188" spans="1:14">
@@ -14582,7 +14576,7 @@
         <v>915</v>
       </c>
       <c r="N188" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="189" spans="1:14">
@@ -14620,7 +14614,7 @@
         <v>915</v>
       </c>
       <c r="N189" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="190" spans="1:14">
@@ -14658,7 +14652,7 @@
         <v>915</v>
       </c>
       <c r="N190" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="191" spans="1:14">
@@ -14696,7 +14690,7 @@
         <v>915</v>
       </c>
       <c r="N191" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="192" spans="1:14">
@@ -14734,7 +14728,7 @@
         <v>915</v>
       </c>
       <c r="N192" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="193" spans="1:14">
@@ -14772,7 +14766,7 @@
         <v>915</v>
       </c>
       <c r="N193" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="194" spans="1:14">
@@ -14812,7 +14806,7 @@
         <v>915</v>
       </c>
       <c r="N194" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="195" spans="1:14">
@@ -14890,7 +14884,7 @@
         <v>915</v>
       </c>
       <c r="N196" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="197" spans="1:14">
@@ -14928,7 +14922,7 @@
         <v>915</v>
       </c>
       <c r="N197" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="198" spans="1:14">
@@ -14966,7 +14960,7 @@
         <v>916</v>
       </c>
       <c r="N198" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="199" spans="1:14">
@@ -15004,7 +14998,7 @@
         <v>915</v>
       </c>
       <c r="N199" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="200" spans="1:14">
@@ -15042,7 +15036,7 @@
         <v>915</v>
       </c>
       <c r="N200" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="201" spans="1:14">
@@ -15080,7 +15074,7 @@
         <v>915</v>
       </c>
       <c r="N201" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="202" spans="1:14">
@@ -15118,7 +15112,7 @@
         <v>915</v>
       </c>
       <c r="N202" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="203" spans="1:14">
@@ -15156,7 +15150,7 @@
         <v>915</v>
       </c>
       <c r="N203" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="204" spans="1:14">
@@ -15194,7 +15188,7 @@
         <v>915</v>
       </c>
       <c r="N204" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="205" spans="1:14">
@@ -15232,7 +15226,7 @@
         <v>915</v>
       </c>
       <c r="N205" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="206" spans="1:14">
@@ -15268,7 +15262,7 @@
         <v>915</v>
       </c>
       <c r="N206" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="207" spans="1:14">
@@ -15304,7 +15298,7 @@
         <v>915</v>
       </c>
       <c r="N207" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="208" spans="1:14">
@@ -15342,7 +15336,7 @@
         <v>915</v>
       </c>
       <c r="N208" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="209" spans="1:14" ht="16.5">
@@ -15364,7 +15358,7 @@
       <c r="F209" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G209" s="224">
+      <c r="G209" s="223">
         <v>50</v>
       </c>
       <c r="H209" s="195" t="s">
@@ -15381,8 +15375,8 @@
       <c r="M209" t="s">
         <v>915</v>
       </c>
-      <c r="N209" s="223" t="s">
-        <v>917</v>
+      <c r="N209" t="s">
+        <v>919</v>
       </c>
     </row>
     <row r="210" spans="1:14" ht="16.5">
@@ -15404,7 +15398,7 @@
       <c r="F210" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G210" s="224">
+      <c r="G210" s="223">
         <v>50</v>
       </c>
       <c r="H210" s="195" t="s">
@@ -15420,7 +15414,7 @@
         <v>915</v>
       </c>
       <c r="N210" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="211" spans="1:14" ht="16.5">
@@ -15442,7 +15436,7 @@
       <c r="F211" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G211" s="224">
+      <c r="G211" s="223">
         <v>50</v>
       </c>
       <c r="H211" s="195"/>
@@ -15458,7 +15452,7 @@
         <v>915</v>
       </c>
       <c r="N211" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="212" spans="1:14" ht="16.5">
@@ -15480,7 +15474,7 @@
       <c r="F212" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G212" s="224">
+      <c r="G212" s="223">
         <v>50</v>
       </c>
       <c r="H212" s="195"/>
@@ -15494,7 +15488,7 @@
         <v>915</v>
       </c>
       <c r="N212" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="213" spans="1:14" ht="16.5">
@@ -15516,7 +15510,7 @@
       <c r="F213" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G213" s="224">
+      <c r="G213" s="223">
         <v>50</v>
       </c>
       <c r="H213" s="195" t="s">
@@ -15534,7 +15528,7 @@
         <v>915</v>
       </c>
       <c r="N213" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="214" spans="1:14" ht="16.5">
@@ -15556,7 +15550,7 @@
       <c r="F214" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G214" s="224">
+      <c r="G214" s="223">
         <v>50</v>
       </c>
       <c r="H214" s="195" t="s">
@@ -15572,7 +15566,7 @@
         <v>915</v>
       </c>
       <c r="N214" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="215" spans="1:14" ht="16.5">
@@ -15594,7 +15588,7 @@
       <c r="F215" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G215" s="224">
+      <c r="G215" s="223">
         <v>50</v>
       </c>
       <c r="H215" s="195" t="s">
@@ -15610,7 +15604,7 @@
         <v>915</v>
       </c>
       <c r="N215" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="216" spans="1:14" ht="16.5">
@@ -15632,7 +15626,7 @@
       <c r="F216" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G216" s="224">
+      <c r="G216" s="223">
         <v>50</v>
       </c>
       <c r="H216" s="195"/>
@@ -15648,7 +15642,7 @@
         <v>915</v>
       </c>
       <c r="N216" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="217" spans="1:14" ht="16.5">
@@ -15670,7 +15664,7 @@
       <c r="F217" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G217" s="224">
+      <c r="G217" s="223">
         <v>50</v>
       </c>
       <c r="H217" s="195" t="s">
@@ -15688,7 +15682,7 @@
         <v>915</v>
       </c>
       <c r="N217" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="218" spans="1:14" ht="16.5">
@@ -15710,7 +15704,7 @@
       <c r="F218" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G218" s="224">
+      <c r="G218" s="223">
         <v>30</v>
       </c>
       <c r="H218" s="195" t="s">
@@ -15728,7 +15722,7 @@
         <v>915</v>
       </c>
       <c r="N218" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="219" spans="1:14" ht="16.5">
@@ -15750,7 +15744,7 @@
       <c r="F219" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G219" s="224">
+      <c r="G219" s="223">
         <v>30</v>
       </c>
       <c r="H219" s="195" t="s">
@@ -15766,7 +15760,7 @@
         <v>915</v>
       </c>
       <c r="N219" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="220" spans="1:14" ht="16.5">
@@ -15788,7 +15782,7 @@
       <c r="F220" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G220" s="224">
+      <c r="G220" s="223">
         <v>30</v>
       </c>
       <c r="H220" s="195" t="s">
@@ -15804,7 +15798,7 @@
         <v>915</v>
       </c>
       <c r="N220" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="221" spans="1:14" ht="16.5">
@@ -15826,7 +15820,7 @@
       <c r="F221" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G221" s="224">
+      <c r="G221" s="223">
         <v>30</v>
       </c>
       <c r="H221" s="195" t="s">
@@ -15842,7 +15836,7 @@
         <v>915</v>
       </c>
       <c r="N221" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="222" spans="1:14" ht="16.5">
@@ -15864,7 +15858,7 @@
       <c r="F222" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G222" s="224">
+      <c r="G222" s="223">
         <v>30</v>
       </c>
       <c r="H222" s="195" t="s">
@@ -15880,7 +15874,7 @@
         <v>915</v>
       </c>
       <c r="N222" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="223" spans="1:14" ht="16.5">
@@ -15902,7 +15896,7 @@
       <c r="F223" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G223" s="224">
+      <c r="G223" s="223">
         <v>30</v>
       </c>
       <c r="H223" s="195" t="s">
@@ -15918,7 +15912,7 @@
         <v>915</v>
       </c>
       <c r="N223" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="224" spans="1:14" ht="16.5">
@@ -15940,7 +15934,7 @@
       <c r="F224" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G224" s="224">
+      <c r="G224" s="223">
         <v>30</v>
       </c>
       <c r="H224" s="195" t="s">
@@ -15956,7 +15950,7 @@
         <v>915</v>
       </c>
       <c r="N224" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="225" spans="1:14" ht="16.5">
@@ -15978,7 +15972,7 @@
       <c r="F225" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G225" s="224">
+      <c r="G225" s="223">
         <v>30</v>
       </c>
       <c r="H225" s="195" t="s">
@@ -15994,7 +15988,7 @@
         <v>915</v>
       </c>
       <c r="N225" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="226" spans="1:14" ht="16.5">
@@ -16016,7 +16010,7 @@
       <c r="F226" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G226" s="224">
+      <c r="G226" s="223">
         <v>30</v>
       </c>
       <c r="H226" s="195" t="s">
@@ -16032,7 +16026,7 @@
         <v>915</v>
       </c>
       <c r="N226" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="227" spans="1:14" ht="16.5">
@@ -16054,7 +16048,7 @@
       <c r="F227" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G227" s="224">
+      <c r="G227" s="223">
         <v>30</v>
       </c>
       <c r="H227" s="195" t="s">
@@ -16070,7 +16064,7 @@
         <v>915</v>
       </c>
       <c r="N227" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="228" spans="1:14" ht="16.5">
@@ -16092,7 +16086,7 @@
       <c r="F228" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G228" s="224">
+      <c r="G228" s="223">
         <v>30</v>
       </c>
       <c r="H228" s="195" t="s">
@@ -16110,7 +16104,7 @@
         <v>915</v>
       </c>
       <c r="N228" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="229" spans="1:14" ht="16.5">
@@ -16132,7 +16126,7 @@
       <c r="F229" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G229" s="224">
+      <c r="G229" s="223">
         <v>46</v>
       </c>
       <c r="H229" s="195"/>
@@ -16148,7 +16142,7 @@
         <v>915</v>
       </c>
       <c r="N229" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="230" spans="1:14" ht="16.5">
@@ -16170,7 +16164,7 @@
       <c r="F230" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G230" s="224">
+      <c r="G230" s="223">
         <v>46</v>
       </c>
       <c r="H230" s="195" t="s">
@@ -16188,7 +16182,7 @@
         <v>915</v>
       </c>
       <c r="N230" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="231" spans="1:14" ht="16.5">
@@ -16210,7 +16204,7 @@
       <c r="F231" s="191" t="s">
         <v>902</v>
       </c>
-      <c r="G231" s="224">
+      <c r="G231" s="223">
         <v>46</v>
       </c>
       <c r="H231" s="196" t="s">
@@ -16228,7 +16222,7 @@
         <v>915</v>
       </c>
       <c r="N231" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="232" spans="1:14" ht="16.5">
@@ -16250,7 +16244,7 @@
       <c r="F232" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G232" s="224">
+      <c r="G232" s="223">
         <v>46</v>
       </c>
       <c r="H232" s="195"/>
@@ -16264,7 +16258,7 @@
         <v>915</v>
       </c>
       <c r="N232" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="233" spans="1:14" ht="16.5">
@@ -16286,7 +16280,7 @@
       <c r="F233" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G233" s="224">
+      <c r="G233" s="223">
         <v>46</v>
       </c>
       <c r="H233" s="195" t="s">
@@ -16304,7 +16298,7 @@
         <v>915</v>
       </c>
       <c r="N233" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="234" spans="1:14" ht="16.5">
@@ -16326,7 +16320,7 @@
       <c r="F234" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G234" s="224">
+      <c r="G234" s="223">
         <v>46</v>
       </c>
       <c r="H234" s="195" t="s">
@@ -16344,7 +16338,7 @@
         <v>915</v>
       </c>
       <c r="N234" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="235" spans="1:14" ht="16.5">
@@ -16366,7 +16360,7 @@
       <c r="F235" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G235" s="224">
+      <c r="G235" s="223">
         <v>46</v>
       </c>
       <c r="H235" s="195" t="s">
@@ -16382,7 +16376,7 @@
         <v>915</v>
       </c>
       <c r="N235" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="236" spans="1:14" ht="16.5">
@@ -16404,7 +16398,7 @@
       <c r="F236" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G236" s="224">
+      <c r="G236" s="223">
         <v>30</v>
       </c>
       <c r="H236" s="195" t="s">
@@ -16422,7 +16416,7 @@
         <v>915</v>
       </c>
       <c r="N236" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="237" spans="1:14" ht="16.5">
@@ -16444,7 +16438,7 @@
       <c r="F237" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G237" s="224">
+      <c r="G237" s="223">
         <v>30</v>
       </c>
       <c r="H237" s="195" t="s">
@@ -16460,7 +16454,7 @@
         <v>915</v>
       </c>
       <c r="N237" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="238" spans="1:14" ht="16.5">
@@ -16482,7 +16476,7 @@
       <c r="F238" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G238" s="224">
+      <c r="G238" s="223">
         <v>30</v>
       </c>
       <c r="H238" s="195" t="s">
@@ -16498,7 +16492,7 @@
         <v>915</v>
       </c>
       <c r="N238" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="239" spans="1:14" ht="16.5">
@@ -16520,7 +16514,7 @@
       <c r="F239" s="191" t="s">
         <v>902</v>
       </c>
-      <c r="G239" s="224">
+      <c r="G239" s="223">
         <v>30</v>
       </c>
       <c r="H239" s="195" t="s">
@@ -16536,7 +16530,7 @@
         <v>915</v>
       </c>
       <c r="N239" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="240" spans="1:14" ht="16.5">
@@ -16558,7 +16552,7 @@
       <c r="F240" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G240" s="224">
+      <c r="G240" s="223">
         <v>30</v>
       </c>
       <c r="H240" s="195" t="s">
@@ -16574,7 +16568,7 @@
         <v>915</v>
       </c>
       <c r="N240" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="241" spans="1:14" ht="16.5">
@@ -16596,7 +16590,7 @@
       <c r="F241" s="191" t="s">
         <v>901</v>
       </c>
-      <c r="G241" s="224">
+      <c r="G241" s="223">
         <v>35</v>
       </c>
       <c r="H241" s="195"/>
@@ -16610,7 +16604,7 @@
         <v>915</v>
       </c>
       <c r="N241" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="242" spans="1:14" ht="16.5">
@@ -16648,7 +16642,7 @@
         <v>915</v>
       </c>
       <c r="N242" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="243" spans="1:14" ht="16.5">
@@ -16686,7 +16680,7 @@
         <v>915</v>
       </c>
       <c r="N243" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="244" spans="1:14">
@@ -16724,7 +16718,7 @@
         <v>915</v>
       </c>
       <c r="N244" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="245" spans="1:14">
@@ -16762,7 +16756,7 @@
         <v>915</v>
       </c>
       <c r="N245" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="246" spans="1:14">
@@ -16802,7 +16796,7 @@
         <v>915</v>
       </c>
       <c r="N246" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="247" spans="1:14">
@@ -16842,7 +16836,7 @@
         <v>915</v>
       </c>
       <c r="N247" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="248" spans="1:14">
@@ -16880,7 +16874,7 @@
         <v>915</v>
       </c>
       <c r="N248" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="249" spans="1:14">
@@ -16918,7 +16912,7 @@
         <v>915</v>
       </c>
       <c r="N249" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="250" spans="1:14">
@@ -16956,7 +16950,7 @@
         <v>915</v>
       </c>
       <c r="N250" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="251" spans="1:14">
@@ -16996,7 +16990,7 @@
         <v>915</v>
       </c>
       <c r="N251" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="252" spans="1:14">
@@ -17036,7 +17030,7 @@
         <v>915</v>
       </c>
       <c r="N252" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="253" spans="1:14">
@@ -17076,7 +17070,7 @@
         <v>915</v>
       </c>
       <c r="N253" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="254" spans="1:14">
@@ -17114,7 +17108,7 @@
         <v>915</v>
       </c>
       <c r="N254" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="255" spans="1:14">
@@ -17152,7 +17146,7 @@
         <v>915</v>
       </c>
       <c r="N255" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="256" spans="1:14">
@@ -17192,7 +17186,7 @@
         <v>915</v>
       </c>
       <c r="N256" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="257" spans="1:14">
@@ -17232,7 +17226,7 @@
         <v>915</v>
       </c>
       <c r="N257" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="258" spans="1:14">
@@ -17272,7 +17266,7 @@
         <v>915</v>
       </c>
       <c r="N258" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="259" spans="1:14">
@@ -17312,7 +17306,7 @@
         <v>915</v>
       </c>
       <c r="N259" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="260" spans="1:14">
@@ -17352,7 +17346,7 @@
         <v>915</v>
       </c>
       <c r="N260" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="261" spans="1:14">
@@ -17390,7 +17384,7 @@
         <v>915</v>
       </c>
       <c r="N261" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="262" spans="1:14">
@@ -17428,7 +17422,7 @@
         <v>915</v>
       </c>
       <c r="N262" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="263" spans="1:14">
@@ -17466,7 +17460,7 @@
         <v>915</v>
       </c>
       <c r="N263" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="264" spans="1:14">
@@ -17504,7 +17498,7 @@
         <v>915</v>
       </c>
       <c r="N264" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="265" spans="1:14">
@@ -17544,7 +17538,7 @@
         <v>915</v>
       </c>
       <c r="N265" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="266" spans="1:14">
@@ -17584,7 +17578,7 @@
         <v>915</v>
       </c>
       <c r="N266" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="267" spans="1:14">
@@ -17620,7 +17614,7 @@
         <v>915</v>
       </c>
       <c r="N267" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="268" spans="1:14">
@@ -17656,7 +17650,7 @@
         <v>915</v>
       </c>
       <c r="N268" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="269" spans="1:14">
@@ -17692,7 +17686,7 @@
         <v>915</v>
       </c>
       <c r="N269" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="270" spans="1:14">
@@ -17730,7 +17724,7 @@
         <v>915</v>
       </c>
       <c r="N270" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="271" spans="1:14">
@@ -17768,7 +17762,7 @@
         <v>915</v>
       </c>
       <c r="N271" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="272" spans="1:14">
@@ -17808,7 +17802,7 @@
         <v>915</v>
       </c>
       <c r="N272" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="273" spans="1:14">
@@ -17848,7 +17842,7 @@
         <v>915</v>
       </c>
       <c r="N273" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="274" spans="1:14">
@@ -17888,7 +17882,7 @@
         <v>915</v>
       </c>
       <c r="N274" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="275" spans="1:14">
@@ -18002,7 +17996,7 @@
         <v>915</v>
       </c>
       <c r="N277" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="278" spans="1:14">
@@ -18040,7 +18034,7 @@
         <v>915</v>
       </c>
       <c r="N278" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="279" spans="1:14">
@@ -18230,7 +18224,7 @@
         <v>915</v>
       </c>
       <c r="N283" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="284" spans="1:14">
@@ -18268,7 +18262,7 @@
         <v>915</v>
       </c>
       <c r="N284" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="285" spans="1:14">
@@ -18306,7 +18300,7 @@
         <v>915</v>
       </c>
       <c r="N285" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="286" spans="1:14">
@@ -18344,7 +18338,7 @@
         <v>915</v>
       </c>
       <c r="N286" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="287" spans="1:14">
@@ -18536,7 +18530,7 @@
         <v>915</v>
       </c>
       <c r="N291" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="292" spans="1:14">
@@ -18576,7 +18570,7 @@
         <v>915</v>
       </c>
       <c r="N292" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="293" spans="1:14">
@@ -18686,7 +18680,7 @@
         <v>915</v>
       </c>
       <c r="N295" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="296" spans="1:14">
@@ -18724,7 +18718,7 @@
         <v>915</v>
       </c>
       <c r="N296" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="297" spans="1:14">
@@ -18762,7 +18756,7 @@
         <v>915</v>
       </c>
       <c r="N297" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="298" spans="1:14">
@@ -18800,7 +18794,7 @@
         <v>915</v>
       </c>
       <c r="N298" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="299" spans="1:14">
@@ -18914,7 +18908,7 @@
         <v>915</v>
       </c>
       <c r="N301" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="302" spans="1:14">
@@ -18952,7 +18946,7 @@
         <v>915</v>
       </c>
       <c r="N302" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="303" spans="1:14">
@@ -18990,7 +18984,7 @@
         <v>915</v>
       </c>
       <c r="N303" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="304" spans="1:14">
@@ -19028,7 +19022,7 @@
         <v>915</v>
       </c>
       <c r="N304" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="305" spans="1:14">
@@ -19064,7 +19058,7 @@
         <v>915</v>
       </c>
       <c r="N305" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="306" spans="1:14">
@@ -19104,7 +19098,7 @@
         <v>915</v>
       </c>
       <c r="N306" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="307" spans="1:14">
@@ -19142,7 +19136,7 @@
         <v>915</v>
       </c>
       <c r="N307" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="308" spans="1:14">
@@ -19370,7 +19364,7 @@
         <v>915</v>
       </c>
       <c r="N313" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="314" spans="1:14">
@@ -19408,7 +19402,7 @@
         <v>915</v>
       </c>
       <c r="N314" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="315" spans="1:14">
@@ -19446,7 +19440,7 @@
         <v>915</v>
       </c>
       <c r="N315" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="316" spans="1:14">
@@ -19484,7 +19478,7 @@
         <v>915</v>
       </c>
       <c r="N316" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="317" spans="1:14">
@@ -19522,7 +19516,7 @@
         <v>915</v>
       </c>
       <c r="N317" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="318" spans="1:14">
@@ -19560,7 +19554,7 @@
         <v>915</v>
       </c>
       <c r="N318" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="319" spans="1:14">
@@ -19598,7 +19592,7 @@
         <v>915</v>
       </c>
       <c r="N319" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="320" spans="1:14">
@@ -19750,7 +19744,7 @@
         <v>915</v>
       </c>
       <c r="N323" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="324" spans="1:14">
@@ -19826,7 +19820,7 @@
         <v>915</v>
       </c>
       <c r="N325" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="326" spans="1:14">
@@ -19864,7 +19858,7 @@
         <v>915</v>
       </c>
       <c r="N326" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="327" spans="1:14">
@@ -20174,7 +20168,7 @@
         <v>915</v>
       </c>
       <c r="N334" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="335" spans="1:14">
@@ -20196,7 +20190,7 @@
       <c r="F335" s="192" t="s">
         <v>901</v>
       </c>
-      <c r="G335" s="225">
+      <c r="G335" s="224">
         <v>56</v>
       </c>
       <c r="H335" s="46"/>
@@ -20212,7 +20206,7 @@
         <v>915</v>
       </c>
       <c r="N335" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="336" spans="1:14">
@@ -20250,7 +20244,7 @@
         <v>915</v>
       </c>
       <c r="N336" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="337" spans="1:14">
@@ -20288,7 +20282,7 @@
         <v>915</v>
       </c>
       <c r="N337" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="338" spans="1:14">
@@ -20326,7 +20320,7 @@
         <v>915</v>
       </c>
       <c r="N338" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="339" spans="1:14">
@@ -20364,7 +20358,7 @@
         <v>915</v>
       </c>
       <c r="N339" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="340" spans="1:14">
@@ -20402,7 +20396,7 @@
         <v>915</v>
       </c>
       <c r="N340" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="341" spans="1:14">
@@ -20440,7 +20434,7 @@
         <v>915</v>
       </c>
       <c r="N341" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="342" spans="1:14">
@@ -20474,7 +20468,7 @@
         <v>915</v>
       </c>
       <c r="N342" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="343" spans="1:14">
@@ -20512,7 +20506,7 @@
         <v>915</v>
       </c>
       <c r="N343" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="344" spans="1:14">
@@ -20550,7 +20544,7 @@
         <v>915</v>
       </c>
       <c r="N344" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="345" spans="1:14">
@@ -20586,7 +20580,7 @@
         <v>915</v>
       </c>
       <c r="N345" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="346" spans="1:14">
@@ -20662,7 +20656,7 @@
         <v>915</v>
       </c>
       <c r="N347" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="348" spans="1:14">
@@ -20700,7 +20694,7 @@
         <v>915</v>
       </c>
       <c r="N348" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="349" spans="1:14">
@@ -20738,7 +20732,7 @@
         <v>915</v>
       </c>
       <c r="N349" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="350" spans="1:14">
@@ -20776,7 +20770,7 @@
         <v>915</v>
       </c>
       <c r="N350" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="351" spans="1:14">
@@ -20814,7 +20808,7 @@
         <v>915</v>
       </c>
       <c r="N351" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="352" spans="1:14">
@@ -20852,7 +20846,7 @@
         <v>915</v>
       </c>
       <c r="N352" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="353" spans="1:14">
@@ -20890,7 +20884,7 @@
         <v>915</v>
       </c>
       <c r="N353" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="354" spans="1:14">
@@ -20928,7 +20922,7 @@
         <v>915</v>
       </c>
       <c r="N354" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="355" spans="1:14">
@@ -20966,7 +20960,7 @@
         <v>915</v>
       </c>
       <c r="N355" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="356" spans="1:14">
@@ -21004,7 +20998,7 @@
         <v>915</v>
       </c>
       <c r="N356" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="357" spans="1:14">
@@ -21042,7 +21036,7 @@
         <v>915</v>
       </c>
       <c r="N357" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="358" spans="1:14">
@@ -21080,7 +21074,7 @@
         <v>916</v>
       </c>
       <c r="N358" t="s">
-        <v>33</v>
+        <v>919</v>
       </c>
     </row>
     <row r="359" spans="1:14">
@@ -21118,7 +21112,7 @@
         <v>915</v>
       </c>
       <c r="N359" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="360" spans="1:14">
@@ -21156,7 +21150,7 @@
         <v>915</v>
       </c>
       <c r="N360" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="361" spans="1:14">
@@ -21194,7 +21188,7 @@
         <v>915</v>
       </c>
       <c r="N361" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="362" spans="1:14">
@@ -21232,7 +21226,7 @@
         <v>915</v>
       </c>
       <c r="N362" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="363" spans="1:14">
@@ -21270,7 +21264,7 @@
         <v>915</v>
       </c>
       <c r="N363" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="364" spans="1:14">
@@ -21308,7 +21302,7 @@
         <v>915</v>
       </c>
       <c r="N364" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="365" spans="1:14">
@@ -21346,7 +21340,7 @@
         <v>915</v>
       </c>
       <c r="N365" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="366" spans="1:14">
@@ -21382,7 +21376,7 @@
         <v>915</v>
       </c>
       <c r="N366" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="367" spans="1:14">
@@ -21420,7 +21414,7 @@
         <v>915</v>
       </c>
       <c r="N367" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="368" spans="1:14">
@@ -21458,7 +21452,7 @@
         <v>915</v>
       </c>
       <c r="N368" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="369" spans="1:14">
@@ -21496,7 +21490,7 @@
         <v>915</v>
       </c>
       <c r="N369" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="370" spans="1:14">
@@ -21534,7 +21528,7 @@
         <v>915</v>
       </c>
       <c r="N370" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="371" spans="1:14">
@@ -21572,7 +21566,7 @@
         <v>915</v>
       </c>
       <c r="N371" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="372" spans="1:14">
@@ -21686,10 +21680,11 @@
         <v>915</v>
       </c>
       <c r="N374" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>